<commit_message>
feat: Add ExcelProcessor class to process and replace specific values in Excel files
- Introduced the ExcelProcessor class with the following functionalities:
  - Read and parse Excel files, extracting headers and data
  - Convert cell data to numeric format, preserving non-numeric data
  - Match columns based on exact or partial string matching
  - Replace values based on specified conditions (greater, less, abs_greater)
  - Log replacements for each matched column
  - Save processed data to a new Excel file and generate a log file

- Usage example included in the class documentation for easy reference

This update allows for flexible processing of Excel files by specifying conditions for value replacement and ensures detailed logging of replacements.
</commit_message>
<xml_diff>
--- a/data/裂缝宽度监测结果.xlsx
+++ b/data/裂缝宽度监测结果.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="68">
   <si>
     <t>测点位置</t>
   </si>
@@ -1434,7 +1434,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1498,7 +1498,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7">
-        <v>-0.011</v>
+        <v>-0.003</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="15"/>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="L2" s="18">
         <f>(F2-G2)-H2</f>
-        <v>0.011</v>
+        <v>0.003</v>
       </c>
       <c r="N2" s="19" t="s">
         <v>14</v>
@@ -1531,7 +1531,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="7">
-        <v>-0.017</v>
+        <v>-0.014</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="15"/>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="L3" s="18">
         <f t="shared" ref="L3:L49" si="1">(F3-G3)-H3</f>
-        <v>0.017</v>
+        <v>0.014</v>
       </c>
       <c r="N3" s="19" t="s">
         <v>16</v>
@@ -1564,7 +1564,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7">
-        <v>-0.007</v>
+        <v>-0.003</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="15"/>
@@ -1575,7 +1575,7 @@
       </c>
       <c r="L4" s="18">
         <f t="shared" si="1"/>
-        <v>0.007</v>
+        <v>0.003</v>
       </c>
       <c r="N4" s="19" t="s">
         <v>18</v>
@@ -1593,17 +1593,15 @@
       <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>20</v>
+      <c r="G5" s="7">
+        <v>0.119</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>20</v>
@@ -1640,7 +1638,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="7">
-        <v>0.008</v>
+        <v>0.004</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="15"/>
@@ -1651,7 +1649,7 @@
       </c>
       <c r="L6" s="18">
         <f t="shared" si="1"/>
-        <v>-0.008</v>
+        <v>-0.004</v>
       </c>
       <c r="O6" s="23"/>
     </row>
@@ -1667,7 +1665,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="7">
-        <v>0.014</v>
+        <v>0.017</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="15"/>
@@ -1678,7 +1676,7 @@
       </c>
       <c r="L7" s="18">
         <f t="shared" si="1"/>
-        <v>-0.014</v>
+        <v>-0.017</v>
       </c>
       <c r="O7" s="23"/>
     </row>
@@ -1690,18 +1688,14 @@
       <c r="C8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1731,7 +1725,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="7">
-        <v>0.001</v>
+        <v>-0.002</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="15"/>
@@ -1742,7 +1736,7 @@
       </c>
       <c r="L9" s="18">
         <f t="shared" si="1"/>
-        <v>-0.001</v>
+        <v>0.002</v>
       </c>
       <c r="O9" s="23"/>
     </row>
@@ -1760,7 +1754,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="7">
-        <v>-0.013</v>
+        <v>-0.002</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="15"/>
@@ -1771,7 +1765,7 @@
       </c>
       <c r="L10" s="18">
         <f t="shared" si="1"/>
-        <v>0.013</v>
+        <v>0.002</v>
       </c>
       <c r="N10" s="19" t="s">
         <v>14</v>
@@ -1793,7 +1787,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="7">
-        <v>0.007</v>
+        <v>0.014</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="15"/>
@@ -1804,7 +1798,7 @@
       </c>
       <c r="L11" s="18">
         <f t="shared" si="1"/>
-        <v>-0.007</v>
+        <v>-0.014</v>
       </c>
       <c r="N11" s="19" t="s">
         <v>16</v>
@@ -1826,7 +1820,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="7">
-        <v>-0.036</v>
+        <v>-0.029</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="15"/>
@@ -1837,7 +1831,7 @@
       </c>
       <c r="L12" s="18">
         <f t="shared" si="1"/>
-        <v>0.036</v>
+        <v>0.029</v>
       </c>
       <c r="N12" s="19" t="s">
         <v>18</v>
@@ -1859,7 +1853,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="7">
-        <v>-0.026</v>
+        <v>-0.021</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="15"/>
@@ -1870,7 +1864,7 @@
       </c>
       <c r="L13" s="18">
         <f t="shared" si="1"/>
-        <v>0.026</v>
+        <v>0.021</v>
       </c>
       <c r="N13" s="19" t="s">
         <v>21</v>
@@ -1888,17 +1882,15 @@
       <c r="C14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>20</v>
+      <c r="G14" s="7">
+        <v>0.646</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>20</v>
@@ -1929,7 +1921,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="7">
-        <v>-0.001</v>
+        <v>0.008</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="15"/>
@@ -1940,7 +1932,7 @@
       </c>
       <c r="L15" s="18">
         <f t="shared" si="1"/>
-        <v>0.001</v>
+        <v>-0.008</v>
       </c>
       <c r="O15" s="23"/>
     </row>
@@ -1952,17 +1944,15 @@
       <c r="C16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>20</v>
+      <c r="G16" s="7">
+        <v>-0.01</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>20</v>
@@ -1988,23 +1978,23 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="7">
-        <v>0.07</v>
+        <v>0.071</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7">
-        <v>0.059</v>
+        <v>0.061</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="15"/>
       <c r="J17" s="16"/>
       <c r="K17" s="17">
         <f t="shared" si="0"/>
-        <v>-0.07</v>
+        <v>-0.071</v>
       </c>
       <c r="L17" s="18">
         <f t="shared" si="1"/>
-        <v>-0.059</v>
+        <v>-0.061</v>
       </c>
       <c r="O17" s="23"/>
     </row>
@@ -2016,17 +2006,15 @@
       <c r="C18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>20</v>
+      <c r="G18" s="7">
+        <v>-0.061</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>20</v>
@@ -2057,7 +2045,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="7">
-        <v>-0.011</v>
+        <v>-0.006</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="15"/>
@@ -2068,7 +2056,7 @@
       </c>
       <c r="L19" s="18">
         <f t="shared" si="1"/>
-        <v>0.011</v>
+        <v>0.006</v>
       </c>
       <c r="O19" s="23"/>
     </row>
@@ -2080,17 +2068,15 @@
       <c r="C20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="D20" s="7"/>
       <c r="E20" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>20</v>
+      <c r="G20" s="7">
+        <v>-0.012</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>20</v>
@@ -2121,7 +2107,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="7">
-        <v>-0.02</v>
+        <v>-0.015</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="15"/>
@@ -2132,7 +2118,7 @@
       </c>
       <c r="L21" s="18">
         <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>0.015</v>
       </c>
       <c r="O21" s="23"/>
     </row>
@@ -2148,7 +2134,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="7">
-        <v>-0.021</v>
+        <v>-0.014</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="15"/>
@@ -2159,7 +2145,7 @@
       </c>
       <c r="L22" s="18">
         <f t="shared" si="1"/>
-        <v>0.021</v>
+        <v>0.014</v>
       </c>
       <c r="O22" s="23"/>
     </row>
@@ -2171,17 +2157,15 @@
       <c r="C23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="D23" s="7"/>
       <c r="E23" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>20</v>
+      <c r="G23" s="7">
+        <v>0.018</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>20</v>
@@ -2212,7 +2196,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="7">
-        <v>-0.022</v>
+        <v>-0.017</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="15"/>
@@ -2223,7 +2207,7 @@
       </c>
       <c r="L24" s="18">
         <f t="shared" si="1"/>
-        <v>0.022</v>
+        <v>0.017</v>
       </c>
       <c r="O24" s="23"/>
     </row>
@@ -2239,7 +2223,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="7">
-        <v>-0.015</v>
+        <v>-0.01</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="15"/>
@@ -2250,7 +2234,7 @@
       </c>
       <c r="L25" s="18">
         <f t="shared" si="1"/>
-        <v>0.015</v>
+        <v>0.01</v>
       </c>
       <c r="O25" s="23"/>
     </row>
@@ -2268,7 +2252,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="7">
-        <v>-0.001</v>
+        <v>0.003</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="15"/>
@@ -2279,7 +2263,7 @@
       </c>
       <c r="L26" s="18">
         <f t="shared" si="1"/>
-        <v>0.001</v>
+        <v>-0.003</v>
       </c>
       <c r="N26" s="19" t="s">
         <v>14</v>
@@ -2301,7 +2285,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="7">
-        <v>-0.027</v>
+        <v>-0.02</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="15"/>
@@ -2312,7 +2296,7 @@
       </c>
       <c r="L27" s="18">
         <f t="shared" si="1"/>
-        <v>0.027</v>
+        <v>0.02</v>
       </c>
       <c r="N27" s="19" t="s">
         <v>16</v>
@@ -2367,7 +2351,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="7">
-        <v>-0.017</v>
+        <v>-0.023</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="15"/>
@@ -2378,7 +2362,7 @@
       </c>
       <c r="L29" s="18">
         <f t="shared" si="1"/>
-        <v>0.017</v>
+        <v>0.023</v>
       </c>
       <c r="N29" s="19" t="s">
         <v>21</v>
@@ -2400,7 +2384,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="7">
-        <v>-0.015</v>
+        <v>-0.006</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="15"/>
@@ -2411,7 +2395,7 @@
       </c>
       <c r="L30" s="18">
         <f t="shared" si="1"/>
-        <v>0.015</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:12">
@@ -2426,7 +2410,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="7">
-        <v>0.022</v>
+        <v>0.02</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="15"/>
@@ -2437,7 +2421,7 @@
       </c>
       <c r="L31" s="18">
         <f t="shared" si="1"/>
-        <v>-0.022</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2448,17 +2432,15 @@
       <c r="C32" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="D32" s="7"/>
       <c r="E32" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="7" t="s">
-        <v>20</v>
+      <c r="G32" s="7">
+        <v>-0.008</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>20</v>
@@ -2488,7 +2470,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="7">
-        <v>0.005</v>
+        <v>0.009</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="15"/>
@@ -2499,7 +2481,7 @@
       </c>
       <c r="L33" s="18">
         <f t="shared" si="1"/>
-        <v>-0.005</v>
+        <v>-0.009</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:12">
@@ -2514,7 +2496,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="7">
-        <v>0.013</v>
+        <v>0.017</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="15"/>
@@ -2525,7 +2507,7 @@
       </c>
       <c r="L34" s="18">
         <f t="shared" si="1"/>
-        <v>-0.013</v>
+        <v>-0.017</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:12">
@@ -2540,7 +2522,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="7">
-        <v>0.016</v>
+        <v>0.015</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="15"/>
@@ -2551,7 +2533,7 @@
       </c>
       <c r="L35" s="18">
         <f t="shared" si="1"/>
-        <v>-0.016</v>
+        <v>-0.015</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:12">
@@ -2588,17 +2570,15 @@
       <c r="C37" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="D37" s="7"/>
       <c r="E37" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G37" s="7" t="s">
-        <v>20</v>
+      <c r="G37" s="7">
+        <v>0.181</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>20</v>
@@ -2628,7 +2608,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="7">
-        <v>0.001</v>
+        <v>0.004</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="15"/>
@@ -2639,7 +2619,7 @@
       </c>
       <c r="L38" s="18">
         <f t="shared" si="1"/>
-        <v>-0.001</v>
+        <v>-0.004</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:12">
@@ -2654,7 +2634,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="7">
-        <v>-0.025</v>
+        <v>-0.022</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="15"/>
@@ -2665,7 +2645,7 @@
       </c>
       <c r="L39" s="18">
         <f t="shared" si="1"/>
-        <v>0.025</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2676,17 +2656,15 @@
       <c r="C40" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="D40" s="7"/>
       <c r="E40" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="7" t="s">
-        <v>20</v>
+      <c r="G40" s="7">
+        <v>-0.343</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>20</v>
@@ -2716,7 +2694,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="7">
-        <v>-0.007</v>
+        <v>-0.015</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="15"/>
@@ -2727,7 +2705,7 @@
       </c>
       <c r="L41" s="18">
         <f t="shared" si="1"/>
-        <v>0.007</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:12">
@@ -2742,7 +2720,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="7">
-        <v>-0.006</v>
+        <v>-0.001</v>
       </c>
       <c r="H42" s="6"/>
       <c r="I42" s="15"/>
@@ -2753,7 +2731,7 @@
       </c>
       <c r="L42" s="18">
         <f t="shared" si="1"/>
-        <v>0.006</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:12">
@@ -2763,23 +2741,23 @@
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="7">
-        <v>0.023</v>
+        <v>0.026</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="7">
-        <v>0.006</v>
+        <v>0.015</v>
       </c>
       <c r="H43" s="6"/>
       <c r="I43" s="15"/>
       <c r="J43" s="16"/>
       <c r="K43" s="17">
         <f t="shared" si="0"/>
-        <v>-0.023</v>
+        <v>-0.026</v>
       </c>
       <c r="L43" s="18">
         <f t="shared" si="1"/>
-        <v>-0.006</v>
+        <v>-0.015</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:12">
@@ -2820,7 +2798,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="7">
-        <v>-0.026</v>
+        <v>-0.032</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="15"/>
@@ -2831,7 +2809,7 @@
       </c>
       <c r="L45" s="18">
         <f t="shared" si="1"/>
-        <v>0.026</v>
+        <v>0.032</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:12">
@@ -2846,7 +2824,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="7">
-        <v>-0.001</v>
+        <v>-0.005</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="15"/>
@@ -2857,7 +2835,7 @@
       </c>
       <c r="L46" s="18">
         <f t="shared" si="1"/>
-        <v>0.001</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:12">
@@ -2872,7 +2850,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="7">
-        <v>-0.01</v>
+        <v>-0.004</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="15"/>
@@ -2883,7 +2861,7 @@
       </c>
       <c r="L47" s="18">
         <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:12">
@@ -2898,7 +2876,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="7">
-        <v>0.005</v>
+        <v>-0.001</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="15"/>
@@ -2909,7 +2887,7 @@
       </c>
       <c r="L48" s="18">
         <f t="shared" si="1"/>
-        <v>-0.005</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="49" ht="15.75" spans="1:12">
@@ -2924,7 +2902,7 @@
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="13">
-        <v>-0.002</v>
+        <v>-0.005</v>
       </c>
       <c r="H49" s="12"/>
       <c r="I49" s="24"/>
@@ -2935,7 +2913,7 @@
       </c>
       <c r="L49" s="27">
         <f t="shared" si="1"/>
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>